<commit_message>
testing surrogates for a smaller example
</commit_message>
<xml_diff>
--- a/pareto/case_studies/strategic_treatment_demo_surrogates.xlsx
+++ b/pareto/case_studies/strategic_treatment_demo_surrogates.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\javal.vyas\Desktop\github\project-pareto_forked\pareto\case_studies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E25E94A-9D86-479B-86C6-902A927BE864}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED0724E9-329D-4AA6-AB18-F30C923E1EF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="905" firstSheet="86" activeTab="90" xr2:uid="{FB8C51AB-905F-4544-9E4B-1F4384FA855C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="905" firstSheet="90" activeTab="90" xr2:uid="{FB8C51AB-905F-4544-9E4B-1F4384FA855C}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="33" r:id="rId1"/>
@@ -1190,7 +1190,7 @@
     <t>recovery</t>
   </si>
   <si>
-    <t>Desalination Treatment Settings</t>
+    <t>Desalination Treatment Settings [kg/s]</t>
   </si>
 </sst>
 </file>
@@ -45826,7 +45826,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B4"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -45874,7 +45874,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>